<commit_message>
linear regression & svm
</commit_message>
<xml_diff>
--- a/Covid/ppkm_mikro_dki.xlsx
+++ b/Covid/ppkm_mikro_dki.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -44,21 +44,6 @@
   </si>
   <si>
     <t>Location_Level</t>
-  </si>
-  <si>
-    <t>New_Cases_per_Million</t>
-  </si>
-  <si>
-    <t>Total_Cases_per_Million</t>
-  </si>
-  <si>
-    <t>New_Death_per_Million</t>
-  </si>
-  <si>
-    <t>Total_Deaths_per_Million</t>
-  </si>
-  <si>
-    <t>Total_Deaths_per_100rb</t>
   </si>
   <si>
     <t>Case_Fatality_Rate</t>
@@ -575,13 +560,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:15">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -624,28 +609,13 @@
       <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>9439</v>
@@ -674,40 +644,25 @@
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2">
-        <v>870.26</v>
-      </c>
-      <c r="M2">
-        <v>55404.85</v>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" t="s">
+        <v>44</v>
       </c>
       <c r="N2">
-        <v>12.63</v>
+        <v>0.87</v>
       </c>
       <c r="O2">
-        <v>816.33</v>
-      </c>
-      <c r="P2">
-        <v>81.63</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>39</v>
-      </c>
-      <c r="R2" t="s">
-        <v>49</v>
-      </c>
-      <c r="S2">
-        <v>0.87</v>
-      </c>
-      <c r="T2">
         <v>1.14</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
         <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>9365</v>
@@ -736,40 +691,25 @@
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3">
-        <v>863.4400000000001</v>
-      </c>
-      <c r="M3">
-        <v>56268.29</v>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
+        <v>45</v>
       </c>
       <c r="N3">
-        <v>13.09</v>
+        <v>0.99</v>
       </c>
       <c r="O3">
-        <v>829.42</v>
-      </c>
-      <c r="P3">
-        <v>82.94</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>39</v>
-      </c>
-      <c r="R3" t="s">
-        <v>50</v>
-      </c>
-      <c r="S3">
-        <v>0.99</v>
-      </c>
-      <c r="T3">
         <v>1.04</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:15">
       <c r="A4" s="1">
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>12974</v>
@@ -798,40 +738,25 @@
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4">
-        <v>1196.19</v>
-      </c>
-      <c r="M4">
-        <v>57464.47</v>
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" t="s">
+        <v>46</v>
       </c>
       <c r="N4">
-        <v>12.54</v>
+        <v>1.39</v>
       </c>
       <c r="O4">
-        <v>841.96</v>
-      </c>
-      <c r="P4">
-        <v>84.2</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>39</v>
-      </c>
-      <c r="R4" t="s">
-        <v>51</v>
-      </c>
-      <c r="S4">
-        <v>1.39</v>
-      </c>
-      <c r="T4">
         <v>0.96</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:15">
       <c r="A5" s="1">
         <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>13111</v>
@@ -860,40 +785,25 @@
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5">
-        <v>1208.82</v>
-      </c>
-      <c r="M5">
-        <v>58673.29</v>
+      <c r="L5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" t="s">
+        <v>47</v>
       </c>
       <c r="N5">
-        <v>12.72</v>
+        <v>1.01</v>
       </c>
       <c r="O5">
-        <v>854.6799999999999</v>
-      </c>
-      <c r="P5">
-        <v>85.47</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>40</v>
-      </c>
-      <c r="R5" t="s">
-        <v>52</v>
-      </c>
-      <c r="S5">
         <v>1.01</v>
       </c>
-      <c r="T5">
-        <v>1.01</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1">
         <v>144</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>12920</v>
@@ -922,40 +832,25 @@
       <c r="K6">
         <v>0</v>
       </c>
-      <c r="L6">
-        <v>1191.21</v>
-      </c>
-      <c r="M6">
-        <v>59864.5</v>
+      <c r="L6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" t="s">
+        <v>48</v>
       </c>
       <c r="N6">
-        <v>8.02</v>
+        <v>0.99</v>
       </c>
       <c r="O6">
-        <v>862.7</v>
-      </c>
-      <c r="P6">
-        <v>86.27</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>41</v>
-      </c>
-      <c r="R6" t="s">
-        <v>53</v>
-      </c>
-      <c r="S6">
-        <v>0.99</v>
-      </c>
-      <c r="T6">
         <v>0.63</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:15">
       <c r="A7" s="1">
         <v>179</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>13133</v>
@@ -984,40 +879,25 @@
       <c r="K7">
         <v>0</v>
       </c>
-      <c r="L7">
-        <v>1210.84</v>
-      </c>
-      <c r="M7">
-        <v>61075.34</v>
+      <c r="L7" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" t="s">
+        <v>49</v>
       </c>
       <c r="N7">
-        <v>4.24</v>
+        <v>1.02</v>
       </c>
       <c r="O7">
-        <v>866.9400000000001</v>
-      </c>
-      <c r="P7">
-        <v>86.69</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>42</v>
-      </c>
-      <c r="R7" t="s">
-        <v>54</v>
-      </c>
-      <c r="S7">
-        <v>1.02</v>
-      </c>
-      <c r="T7">
         <v>0.53</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:15">
       <c r="A8" s="1">
         <v>214</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>14622</v>
@@ -1046,40 +926,25 @@
       <c r="K8">
         <v>0</v>
       </c>
-      <c r="L8">
-        <v>1348.13</v>
-      </c>
-      <c r="M8">
-        <v>62423.47</v>
+      <c r="L8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" t="s">
+        <v>50</v>
       </c>
       <c r="N8">
-        <v>12.35</v>
+        <v>1.11</v>
       </c>
       <c r="O8">
-        <v>879.3</v>
-      </c>
-      <c r="P8">
-        <v>87.93000000000001</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>43</v>
-      </c>
-      <c r="R8" t="s">
-        <v>55</v>
-      </c>
-      <c r="S8">
-        <v>1.11</v>
-      </c>
-      <c r="T8">
         <v>2.91</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:15">
       <c r="A9" s="1">
         <v>249</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>12183</v>
@@ -1108,40 +973,25 @@
       <c r="K9">
         <v>0</v>
       </c>
-      <c r="L9">
-        <v>1123.26</v>
-      </c>
-      <c r="M9">
-        <v>63546.73</v>
+      <c r="L9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" t="s">
+        <v>51</v>
       </c>
       <c r="N9">
-        <v>6.27</v>
+        <v>0.83</v>
       </c>
       <c r="O9">
-        <v>885.5700000000001</v>
-      </c>
-      <c r="P9">
-        <v>88.56</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>44</v>
-      </c>
-      <c r="R9" t="s">
-        <v>56</v>
-      </c>
-      <c r="S9">
-        <v>0.83</v>
-      </c>
-      <c r="T9">
         <v>0.51</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:15">
       <c r="A10" s="1">
         <v>284</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>12669</v>
@@ -1170,40 +1020,25 @@
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10">
-        <v>1168.06</v>
-      </c>
-      <c r="M10">
-        <v>64714.79</v>
+      <c r="L10" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" t="s">
+        <v>52</v>
       </c>
       <c r="N10">
-        <v>5.81</v>
+        <v>1.04</v>
       </c>
       <c r="O10">
-        <v>891.38</v>
-      </c>
-      <c r="P10">
-        <v>89.14</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R10" t="s">
-        <v>57</v>
-      </c>
-      <c r="S10">
-        <v>1.04</v>
-      </c>
-      <c r="T10">
         <v>0.93</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:15">
       <c r="A11" s="1">
         <v>319</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C11">
         <v>12691</v>
@@ -1232,40 +1067,25 @@
       <c r="K11">
         <v>0</v>
       </c>
-      <c r="L11">
-        <v>1170.09</v>
-      </c>
-      <c r="M11">
-        <v>65884.88</v>
+      <c r="L11" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" t="s">
+        <v>53</v>
       </c>
       <c r="N11">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="O11">
-        <v>904.38</v>
-      </c>
-      <c r="P11">
-        <v>90.44</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>46</v>
-      </c>
-      <c r="R11" t="s">
-        <v>58</v>
-      </c>
-      <c r="S11">
-        <v>1</v>
-      </c>
-      <c r="T11">
         <v>2.24</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:15">
       <c r="A12" s="1">
         <v>354</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C12">
         <v>12416</v>
@@ -1294,40 +1114,25 @@
       <c r="K12">
         <v>0</v>
       </c>
-      <c r="L12">
-        <v>1144.74</v>
-      </c>
-      <c r="M12">
-        <v>67029.62</v>
+      <c r="L12" t="s">
+        <v>41</v>
+      </c>
+      <c r="M12" t="s">
+        <v>54</v>
       </c>
       <c r="N12">
-        <v>12.17</v>
+        <v>0.98</v>
       </c>
       <c r="O12">
-        <v>916.55</v>
-      </c>
-      <c r="P12">
-        <v>91.65000000000001</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>46</v>
-      </c>
-      <c r="R12" t="s">
-        <v>59</v>
-      </c>
-      <c r="S12">
-        <v>0.98</v>
-      </c>
-      <c r="T12">
         <v>0.9399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:15">
       <c r="A13" s="1">
         <v>389</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C13">
         <v>10168</v>
@@ -1356,40 +1161,25 @@
       <c r="K13">
         <v>0</v>
       </c>
-      <c r="L13">
-        <v>937.48</v>
-      </c>
-      <c r="M13">
-        <v>67967.10000000001</v>
+      <c r="L13" t="s">
+        <v>42</v>
+      </c>
+      <c r="M13" t="s">
+        <v>55</v>
       </c>
       <c r="N13">
-        <v>6.18</v>
+        <v>0.82</v>
       </c>
       <c r="O13">
-        <v>922.72</v>
-      </c>
-      <c r="P13">
-        <v>92.27</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>47</v>
-      </c>
-      <c r="R13" t="s">
-        <v>60</v>
-      </c>
-      <c r="S13">
-        <v>0.82</v>
-      </c>
-      <c r="T13">
         <v>0.51</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:15">
       <c r="A14" s="1">
         <v>424</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C14">
         <v>9129</v>
@@ -1418,40 +1208,25 @@
       <c r="K14">
         <v>0</v>
       </c>
-      <c r="L14">
-        <v>841.6799999999999</v>
-      </c>
-      <c r="M14">
-        <v>68808.78</v>
+      <c r="L14" t="s">
+        <v>42</v>
+      </c>
+      <c r="M14" t="s">
+        <v>56</v>
       </c>
       <c r="N14">
-        <v>14.57</v>
+        <v>0.9</v>
       </c>
       <c r="O14">
-        <v>937.29</v>
-      </c>
-      <c r="P14">
-        <v>93.73</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>47</v>
-      </c>
-      <c r="R14" t="s">
-        <v>61</v>
-      </c>
-      <c r="S14">
-        <v>0.9</v>
-      </c>
-      <c r="T14">
         <v>2.36</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:15">
       <c r="A15" s="1">
         <v>459</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C15">
         <v>5000</v>
@@ -1480,40 +1255,25 @@
       <c r="K15">
         <v>0</v>
       </c>
-      <c r="L15">
-        <v>460.99</v>
-      </c>
-      <c r="M15">
-        <v>69269.77</v>
+      <c r="L15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" t="s">
+        <v>49</v>
       </c>
       <c r="N15">
-        <v>23.05</v>
+        <v>0.55</v>
       </c>
       <c r="O15">
-        <v>960.34</v>
-      </c>
-      <c r="P15">
-        <v>96.03</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>44</v>
-      </c>
-      <c r="R15" t="s">
-        <v>54</v>
-      </c>
-      <c r="S15">
-        <v>0.55</v>
-      </c>
-      <c r="T15">
         <v>1.58</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:15">
       <c r="A16" s="1">
         <v>494</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C16">
         <v>6213</v>
@@ -1542,40 +1302,25 @@
       <c r="K16">
         <v>0</v>
       </c>
-      <c r="L16">
-        <v>572.83</v>
-      </c>
-      <c r="M16">
-        <v>69842.60000000001</v>
+      <c r="L16" t="s">
+        <v>38</v>
+      </c>
+      <c r="M16" t="s">
+        <v>57</v>
       </c>
       <c r="N16">
-        <v>24.71</v>
+        <v>1.24</v>
       </c>
       <c r="O16">
-        <v>985.05</v>
-      </c>
-      <c r="P16">
-        <v>98.51000000000001</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>43</v>
-      </c>
-      <c r="R16" t="s">
-        <v>62</v>
-      </c>
-      <c r="S16">
-        <v>1.24</v>
-      </c>
-      <c r="T16">
         <v>1.07</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:15">
       <c r="A17" s="1">
         <v>529</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C17">
         <v>5904</v>
@@ -1604,40 +1349,25 @@
       <c r="K17">
         <v>0</v>
       </c>
-      <c r="L17">
-        <v>544.34</v>
-      </c>
-      <c r="M17">
-        <v>70386.94</v>
+      <c r="L17" t="s">
+        <v>38</v>
+      </c>
+      <c r="M17" t="s">
+        <v>58</v>
       </c>
       <c r="N17">
-        <v>8.76</v>
+        <v>0.95</v>
       </c>
       <c r="O17">
-        <v>993.8099999999999</v>
-      </c>
-      <c r="P17">
-        <v>99.38</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>43</v>
-      </c>
-      <c r="R17" t="s">
-        <v>63</v>
-      </c>
-      <c r="S17">
-        <v>0.95</v>
-      </c>
-      <c r="T17">
         <v>0.35</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:15">
       <c r="A18" s="1">
         <v>564</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>7060</v>
@@ -1666,40 +1396,25 @@
       <c r="K18">
         <v>0</v>
       </c>
-      <c r="L18">
-        <v>650.92</v>
-      </c>
-      <c r="M18">
-        <v>71037.87</v>
+      <c r="L18" t="s">
+        <v>37</v>
+      </c>
+      <c r="M18" t="s">
+        <v>59</v>
       </c>
       <c r="N18">
-        <v>17.98</v>
+        <v>1.2</v>
       </c>
       <c r="O18">
-        <v>1011.79</v>
-      </c>
-      <c r="P18">
-        <v>101.18</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>42</v>
-      </c>
-      <c r="R18" t="s">
-        <v>64</v>
-      </c>
-      <c r="S18">
-        <v>1.2</v>
-      </c>
-      <c r="T18">
         <v>2.05</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:15">
       <c r="A19" s="1">
         <v>599</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C19">
         <v>8033</v>
@@ -1728,40 +1443,25 @@
       <c r="K19">
         <v>0</v>
       </c>
-      <c r="L19">
-        <v>740.63</v>
-      </c>
-      <c r="M19">
-        <v>71778.5</v>
+      <c r="L19" t="s">
+        <v>43</v>
+      </c>
+      <c r="M19" t="s">
+        <v>60</v>
       </c>
       <c r="N19">
-        <v>14.48</v>
+        <v>1.14</v>
       </c>
       <c r="O19">
-        <v>1026.26</v>
-      </c>
-      <c r="P19">
-        <v>102.63</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>48</v>
-      </c>
-      <c r="R19" t="s">
-        <v>65</v>
-      </c>
-      <c r="S19">
-        <v>1.14</v>
-      </c>
-      <c r="T19">
         <v>0.8100000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:15">
       <c r="A20" s="1">
         <v>634</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>8359</v>
@@ -1790,40 +1490,25 @@
       <c r="K20">
         <v>0</v>
       </c>
-      <c r="L20">
-        <v>770.6900000000001</v>
-      </c>
-      <c r="M20">
-        <v>72549.19</v>
+      <c r="L20" t="s">
+        <v>43</v>
+      </c>
+      <c r="M20" t="s">
+        <v>61</v>
       </c>
       <c r="N20">
-        <v>13.92</v>
+        <v>1.04</v>
       </c>
       <c r="O20">
-        <v>1040.19</v>
-      </c>
-      <c r="P20">
-        <v>104.02</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>48</v>
-      </c>
-      <c r="R20" t="s">
-        <v>66</v>
-      </c>
-      <c r="S20">
-        <v>1.04</v>
-      </c>
-      <c r="T20">
         <v>0.96</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:15">
       <c r="A21" s="1">
         <v>669</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C21">
         <v>5394</v>
@@ -1852,31 +1537,16 @@
       <c r="K21">
         <v>0</v>
       </c>
-      <c r="L21">
-        <v>497.32</v>
-      </c>
-      <c r="M21">
-        <v>73046.50999999999</v>
+      <c r="L21" t="s">
+        <v>36</v>
+      </c>
+      <c r="M21" t="s">
+        <v>62</v>
       </c>
       <c r="N21">
-        <v>14.48</v>
+        <v>0.65</v>
       </c>
       <c r="O21">
-        <v>1054.66</v>
-      </c>
-      <c r="P21">
-        <v>105.47</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>41</v>
-      </c>
-      <c r="R21" t="s">
-        <v>67</v>
-      </c>
-      <c r="S21">
-        <v>0.65</v>
-      </c>
-      <c r="T21">
         <v>1.04</v>
       </c>
     </row>

</xml_diff>